<commit_message>
Update parameter files with WEP scaling and WFF_or_Ben
</commit_message>
<xml_diff>
--- a/inst/MFTC_calculator/App_Parameters/HYEFU23_TY14.xlsx
+++ b/inst/MFTC_calculator/App_Parameters/HYEFU23_TY14.xlsx
@@ -8,12 +8,25 @@
   <sheets>
     <sheet name="Parameters" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="195">
   <si>
     <t>Parameter</t>
   </si>
@@ -288,6 +301,21 @@
     <t>Independent Earner Tax Credit, minimum bound on earned income to determine eligibility</t>
   </si>
   <si>
+    <t>MFTC_WEP_scaling</t>
+  </si>
+  <si>
+    <t>WFF_or_Benefit</t>
+  </si>
+  <si>
+    <t>How should the Winter Energy Payment be scaled? Average week = 1, Winter week = 12/5, Summer week = 0</t>
+  </si>
+  <si>
+    <t>What work decision should we assume? Go off-benefit and receive IWTC = "WFF", stay on-benefit = "Benefit", or whichever gives a higher net income = "Max"</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
     <t xml:space="preserve">Parameter</t>
   </si>
   <si>
@@ -571,6 +599,18 @@
   </si>
   <si>
     <t xml:space="preserve">[['0'; '0.105']; ['14000'; '0.175']; ['48000'; '0.3']; ['70000'; '0.33']]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MFTC_WEP_scaling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WFF_or_Benefit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max</t>
   </si>
 </sst>
 </file>
@@ -656,7 +696,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -690,6 +730,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1009,11 +1052,11 @@
       <c r="D1" s="14"/>
     </row>
     <row r="2" ht="17.149999999999999" customHeight="1">
-      <c r="B2" s="19" t="s">
-        <v>91</v>
+      <c r="B2" s="20" t="s">
+        <v>96</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>47</v>
@@ -1021,43 +1064,43 @@
     </row>
     <row r="3">
       <c r="B3" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4">
-      <c r="B4" s="15" t="s">
-        <v>95</v>
+      <c r="B4" s="16" t="s">
+        <v>100</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>96</v>
+        <v>101</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="5">
-      <c r="B5" s="16" t="s">
-        <v>97</v>
+      <c r="B5" s="17" t="s">
+        <v>102</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="6">
-      <c r="B6" s="18" t="s">
-        <v>99</v>
+      <c r="B6" s="19" t="s">
+        <v>104</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>66</v>
@@ -1065,10 +1108,10 @@
     </row>
     <row r="7">
       <c r="B7" s="10" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>49</v>
@@ -1076,10 +1119,10 @@
     </row>
     <row r="8">
       <c r="B8" s="10" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>49</v>
@@ -1087,10 +1130,10 @@
     </row>
     <row r="9">
       <c r="B9" s="10" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>49</v>
@@ -1098,10 +1141,10 @@
     </row>
     <row r="10">
       <c r="B10" s="10" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>49</v>
@@ -1109,10 +1152,10 @@
     </row>
     <row r="11">
       <c r="B11" s="10" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>49</v>
@@ -1120,10 +1163,10 @@
     </row>
     <row r="12">
       <c r="B12" s="10" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>49</v>
@@ -1131,10 +1174,10 @@
     </row>
     <row r="13">
       <c r="B13" s="10" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>49</v>
@@ -1142,10 +1185,10 @@
     </row>
     <row r="14">
       <c r="B14" s="10" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>49</v>
@@ -1153,10 +1196,10 @@
     </row>
     <row r="15">
       <c r="B15" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>116</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>111</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>49</v>
@@ -1164,10 +1207,10 @@
     </row>
     <row r="16">
       <c r="B16" s="10" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>49</v>
@@ -1175,10 +1218,10 @@
     </row>
     <row r="17">
       <c r="B17" s="10" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>49</v>
@@ -1186,10 +1229,10 @@
     </row>
     <row r="18">
       <c r="B18" s="10" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>49</v>
@@ -1197,10 +1240,10 @@
     </row>
     <row r="19">
       <c r="B19" s="10" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>49</v>
@@ -1208,32 +1251,32 @@
     </row>
     <row r="20">
       <c r="B20" s="10" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="21">
-      <c r="B21" s="17" t="s">
-        <v>127</v>
+      <c r="B21" s="18" t="s">
+        <v>132</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="22">
-      <c r="B22" s="15" t="s">
-        <v>129</v>
+      <c r="B22" s="16" t="s">
+        <v>134</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="D22" s="4" t="s">
         <v>51</v>
@@ -1241,10 +1284,10 @@
     </row>
     <row r="23">
       <c r="B23" s="11" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>51</v>
@@ -1252,10 +1295,10 @@
     </row>
     <row r="24">
       <c r="B24" s="11" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>51</v>
@@ -1263,10 +1306,10 @@
     </row>
     <row r="25">
       <c r="B25" s="11" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>51</v>
@@ -1274,10 +1317,10 @@
     </row>
     <row r="26">
       <c r="B26" s="11" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>51</v>
@@ -1285,21 +1328,21 @@
     </row>
     <row r="27">
       <c r="B27" s="11" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="28">
-      <c r="B28" s="18" t="s">
-        <v>141</v>
+      <c r="B28" s="19" t="s">
+        <v>146</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>52</v>
@@ -1307,21 +1350,21 @@
     </row>
     <row r="29">
       <c r="B29" s="10" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C29" s="7" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="30">
-      <c r="B30" s="17" t="s">
-        <v>144</v>
+      <c r="B30" s="18" t="s">
+        <v>149</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>50</v>
@@ -1329,32 +1372,32 @@
     </row>
     <row r="31">
       <c r="B31" s="11" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="32">
-      <c r="B32" s="16" t="s">
-        <v>147</v>
+      <c r="B32" s="17" t="s">
+        <v>152</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="33">
-      <c r="B33" s="15" t="s">
-        <v>148</v>
+      <c r="B33" s="16" t="s">
+        <v>153</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>78</v>
@@ -1362,10 +1405,10 @@
     </row>
     <row r="34">
       <c r="B34" s="11" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D34" s="9" t="s">
         <v>77</v>
@@ -1373,10 +1416,10 @@
     </row>
     <row r="35">
       <c r="B35" s="11" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>55</v>
@@ -1384,21 +1427,21 @@
     </row>
     <row r="36">
       <c r="B36" s="11" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="D36" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="37">
-      <c r="B37" s="18" t="s">
-        <v>155</v>
+      <c r="B37" s="19" t="s">
+        <v>160</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>68</v>
@@ -1406,10 +1449,10 @@
     </row>
     <row r="38">
       <c r="B38" s="10" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>69</v>
@@ -1417,10 +1460,10 @@
     </row>
     <row r="39">
       <c r="B39" s="10" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>87</v>
@@ -1428,10 +1471,10 @@
     </row>
     <row r="40">
       <c r="B40" s="10" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>70</v>
@@ -1439,10 +1482,10 @@
     </row>
     <row r="41">
       <c r="B41" s="10" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="C41" s="7" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>71</v>
@@ -1450,10 +1493,10 @@
     </row>
     <row r="42">
       <c r="B42" s="10" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D42" s="7" t="s">
         <v>57</v>
@@ -1461,10 +1504,10 @@
     </row>
     <row r="43">
       <c r="B43" s="10" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>59</v>
@@ -1472,10 +1515,10 @@
     </row>
     <row r="44">
       <c r="B44" s="10" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>58</v>
@@ -1483,43 +1526,43 @@
     </row>
     <row r="45">
       <c r="B45" s="10" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="D45" s="7" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="46">
-      <c r="B46" s="17" t="s">
-        <v>169</v>
+      <c r="B46" s="18" t="s">
+        <v>174</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="D46" s="8" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="47">
-      <c r="B47" s="16" t="s">
-        <v>171</v>
+      <c r="B47" s="17" t="s">
+        <v>176</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="48">
-      <c r="B48" s="18" t="s">
-        <v>173</v>
+      <c r="B48" s="19" t="s">
+        <v>178</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>60</v>
@@ -1527,32 +1570,32 @@
     </row>
     <row r="49">
       <c r="B49" s="10" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D49" s="7" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="50">
-      <c r="B50" s="17" t="s">
-        <v>176</v>
+      <c r="B50" s="18" t="s">
+        <v>181</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="51">
-      <c r="B51" s="15" t="s">
-        <v>177</v>
+      <c r="B51" s="16" t="s">
+        <v>182</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>74</v>
@@ -1560,10 +1603,10 @@
     </row>
     <row r="52">
       <c r="B52" s="11" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="D52" s="9" t="s">
         <v>90</v>
@@ -1571,21 +1614,21 @@
     </row>
     <row r="53">
       <c r="B53" s="11" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="54">
-      <c r="B54" s="16" t="s">
-        <v>183</v>
+      <c r="B54" s="17" t="s">
+        <v>188</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>73</v>
@@ -1593,13 +1636,35 @@
     </row>
     <row r="55">
       <c r="B55" s="12" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="C55" s="13" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="D55" s="13" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="C56" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="C57" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>